<commit_message>
Added more user creation cases
</commit_message>
<xml_diff>
--- a/TestData/IMIassist_Automation_TestData.xlsx
+++ b/TestData/IMIassist_Automation_TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IMI_Automation\IMI_Automation_files\Staging_IMIAssist_Automation\IMIAssist_Automtion\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IMI_Automation\IMIAssist_Automtion\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E717AD1-DADC-492A-A647-F7CA779B3E79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="9" activeTab="13"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="11" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login_testdata" sheetId="1" r:id="rId1"/>
@@ -26,18 +27,27 @@
     <sheet name="Invalidusername" sheetId="5" r:id="rId12"/>
     <sheet name="Invalidpassword" sheetId="6" r:id="rId13"/>
     <sheet name="IMIA_Dashboard" sheetId="15" r:id="rId14"/>
+    <sheet name="AdminSettings_User" sheetId="16" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="172">
   <si>
     <t>URL</t>
   </si>
@@ -461,12 +471,105 @@
   </si>
   <si>
     <t>InvalidPassword</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Success_or_Error?</t>
+  </si>
+  <si>
+    <t>FirstName is Empty</t>
+  </si>
+  <si>
+    <t>Special chars in FirstName</t>
+  </si>
+  <si>
+    <t>Select Role Empty</t>
+  </si>
+  <si>
+    <t>Expected_Msg_FieldLevel</t>
+  </si>
+  <si>
+    <t>Expected_Msg_Header</t>
+  </si>
+  <si>
+    <t>TestType</t>
+  </si>
+  <si>
+    <t>Negative</t>
+  </si>
+  <si>
+    <t>Possitive</t>
+  </si>
+  <si>
+    <t>Ravi</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Specialty Admin</t>
+  </si>
+  <si>
+    <t>Bolla</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>r@v8</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Please Enter First Name</t>
+  </si>
+  <si>
+    <t>Empty Email</t>
+  </si>
+  <si>
+    <t>Please Enter Email</t>
+  </si>
+  <si>
+    <t>rav</t>
+  </si>
+  <si>
+    <t>Please select user's role</t>
+  </si>
+  <si>
+    <t>Please enter letters only</t>
+  </si>
+  <si>
+    <t>Successful Creation_User</t>
+  </si>
+  <si>
+    <t>Successful Creation_SpAdmin</t>
+  </si>
+  <si>
+    <t>User created successfully. Email sent to user with credentials.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy&quot; &quot;hh&quot;:&quot;mm"/>
   </numFmts>
@@ -955,21 +1058,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -980,7 +1083,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>117</v>
       </c>
@@ -993,8 +1096,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2" location="!/registration/login" display="https://stg.imiassist.ai/agent/ - !/registration/login"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId2" location="!/registration/login" display="https://stg.imiassist.ai/agent/ - !/registration/login" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -1002,23 +1105,23 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1035,7 +1138,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>117</v>
       </c>
@@ -1054,36 +1157,37 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="A2" r:id="rId4" location="!/registration/login"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
+    <hyperlink ref="A2" r:id="rId4" location="!/registration/login" xr:uid="{00000000-0004-0000-0900-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.54296875" customWidth="1"/>
-    <col min="5" max="5" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1112,7 +1216,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>117</v>
       </c>
@@ -1143,9 +1247,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2" location="!/registration/login"/>
-    <hyperlink ref="F2" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId2" location="!/registration/login" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId3" xr:uid="{00000000-0004-0000-0A00-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId4"/>
@@ -1153,21 +1257,21 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1178,7 +1282,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>117</v>
       </c>
@@ -1191,30 +1295,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="A2" r:id="rId3" location="!/registration/login"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0B00-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId3" location="!/registration/login" xr:uid="{00000000-0004-0000-0B00-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.26953125" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1225,7 +1330,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>117</v>
       </c>
@@ -1238,30 +1343,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2"/>
-    <hyperlink ref="A2" r:id="rId3" location="!/registration/login"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0C00-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0C00-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId3" location="!/registration/login" xr:uid="{00000000-0004-0000-0C00-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
         <v>19</v>
       </c>
@@ -1272,7 +1378,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>117</v>
       </c>
@@ -1285,32 +1391,266 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2" location="!/registration/login"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId2" location="!/registration/login" xr:uid="{00000000-0004-0000-0D00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E76F3CF-40A2-4FC7-97CF-E7F60422CA6B}">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E2" t="str">
+        <f ca="1">"Testinguser"&amp;TEXT(NOW(),"ddmmhh")&amp;"@gmail.com"</f>
+        <v>Testinguser091019@gmail.com</v>
+      </c>
+      <c r="G2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D3" t="s">
+        <v>155</v>
+      </c>
+      <c r="E3" t="str">
+        <f ca="1">"Testinguser"&amp;TEXT(NOW(),"ddmmhh")&amp;"@gmail.com"</f>
+        <v>Testinguser091019@gmail.com</v>
+      </c>
+      <c r="F3" t="s">
+        <v>156</v>
+      </c>
+      <c r="G3" t="s">
+        <v>161</v>
+      </c>
+      <c r="I3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D4" t="s">
+        <v>155</v>
+      </c>
+      <c r="E4" t="str">
+        <f ca="1">"Testinguser"&amp;TEXT(NOW(),"ddmmhh")&amp;"@gmail.com"</f>
+        <v>Testinguser091019@gmail.com</v>
+      </c>
+      <c r="F4" t="s">
+        <v>156</v>
+      </c>
+      <c r="G4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" t="s">
+        <v>154</v>
+      </c>
+      <c r="D5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F5" t="s">
+        <v>156</v>
+      </c>
+      <c r="G5" t="s">
+        <v>161</v>
+      </c>
+      <c r="I5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D6" t="s">
+        <v>155</v>
+      </c>
+      <c r="E6" t="s">
+        <v>166</v>
+      </c>
+      <c r="F6" t="s">
+        <v>156</v>
+      </c>
+      <c r="G6" t="s">
+        <v>161</v>
+      </c>
+      <c r="H6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B7" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D7" t="s">
+        <v>155</v>
+      </c>
+      <c r="E7" t="str">
+        <f>"Testinguser0910111@gmail.com"</f>
+        <v>Testinguser0910111@gmail.com</v>
+      </c>
+      <c r="F7" t="s">
+        <v>156</v>
+      </c>
+      <c r="G7" t="s">
+        <v>162</v>
+      </c>
+      <c r="I7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D8" t="s">
+        <v>159</v>
+      </c>
+      <c r="E8" t="str">
+        <f ca="1">"Testingspa"&amp;TEXT(NOW(),"ddmmhh")&amp;"@gmail.com"</f>
+        <v>Testingspa091019@gmail.com</v>
+      </c>
+      <c r="F8" t="s">
+        <v>157</v>
+      </c>
+      <c r="G8" t="s">
+        <v>162</v>
+      </c>
+      <c r="I8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1327,7 +1667,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>117</v>
       </c>
@@ -1346,36 +1686,37 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="A2" r:id="rId4" location="!/registration/login" display="https://stg.imiassist.ai/agent/ - !/registration/login"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="A2" r:id="rId4" location="!/registration/login" display="https://stg.imiassist.ai/agent/ - !/registration/login" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="18.54296875" style="8" customWidth="1"/>
+    <col min="1" max="1" width="49.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="8" customWidth="1"/>
     <col min="5" max="5" width="22" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.1796875" style="8"/>
-    <col min="8" max="8" width="33.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="8"/>
+    <col min="6" max="7" width="9.140625" style="8"/>
+    <col min="8" max="8" width="33.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1404,7 +1745,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>117</v>
       </c>
@@ -1435,8 +1776,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2" location="!/registration/login" display="https://stg.imiassist.ai/agent/ - !/registration/login"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId2" location="!/registration/login" display="https://stg.imiassist.ai/agent/ - !/registration/login" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId3"/>
@@ -1444,39 +1785,39 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47" style="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.81640625" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.81640625" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.7265625" style="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.54296875" style="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.453125" style="27" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.453125" style="27" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7265625" style="27"/>
-    <col min="9" max="9" width="13.81640625" style="27" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.453125" style="27" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.1796875" style="27" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.81640625" style="27" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.453125" style="27" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.26953125" style="27" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.7265625" style="27" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.453125" style="27" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.26953125" style="27" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="35.08984375" style="27" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.81640625" style="27" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="26.08984375" style="27" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.7265625" style="27"/>
+    <col min="2" max="2" width="22.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="27"/>
+    <col min="9" max="9" width="13.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" style="27" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.7109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.28515625" style="27" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="35.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="26.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.7109375" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>19</v>
       </c>
@@ -1541,7 +1882,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="30" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" s="30" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>117</v>
       </c>
@@ -1580,7 +1921,7 @@
       </c>
       <c r="M2" s="32">
         <f ca="1">NOW()+3</f>
-        <v>44114.653952314817</v>
+        <v>44116.821882060183</v>
       </c>
       <c r="N2" s="30" t="s">
         <v>11</v>
@@ -1607,19 +1948,19 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B6" s="30" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="O2" r:id="rId4"/>
-    <hyperlink ref="J2" r:id="rId5"/>
-    <hyperlink ref="A2" r:id="rId6" location="!/registration/login"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="O2" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="J2" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="A2" r:id="rId6" location="!/registration/login" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId7"/>
@@ -1627,24 +1968,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="35">
         <f>DATE(2020,9,7)+1</f>
         <v>44082</v>
@@ -1652,39 +1993,40 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.453125" style="21" customWidth="1"/>
-    <col min="3" max="3" width="28.26953125" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.453125" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7265625" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" style="21"/>
-    <col min="7" max="7" width="25.1796875" style="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7265625" style="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.26953125" style="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.1796875" style="21"/>
-    <col min="11" max="11" width="22.26953125" style="21" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.453125" style="21" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.1796875" style="21"/>
-    <col min="14" max="14" width="23.453125" style="21" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="30.453125" style="21" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.453125" style="21" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.1796875" style="21"/>
+    <col min="1" max="1" width="14.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" style="21" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="21"/>
+    <col min="7" max="7" width="25.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="21"/>
+    <col min="11" max="11" width="22.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="21"/>
+    <col min="14" max="14" width="23.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>85</v>
       </c>
@@ -1734,7 +2076,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>86</v>
       </c>
@@ -1787,8 +2129,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="G2" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="G2" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -1796,21 +2138,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>120</v>
       </c>
@@ -1826,45 +2168,46 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1"/>
-    <hyperlink ref="D1" r:id="rId2"/>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="D1" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.26953125" style="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" style="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" style="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" style="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.453125" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.54296875" style="18" customWidth="1"/>
-    <col min="7" max="7" width="23.453125" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.81640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7265625" style="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.7265625" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.5703125" style="18" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.7109375" style="18" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" style="18" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.453125" style="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.54296875" style="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.453125" style="18" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.453125" style="18" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.1796875" style="18" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.1796875" style="19" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="42.54296875" style="18" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.1796875" style="18"/>
+    <col min="12" max="12" width="23.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="42.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="13" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" s="13" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>44</v>
       </c>
@@ -1923,7 +2266,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="15" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>52</v>
       </c>
@@ -1978,7 +2321,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
@@ -1986,22 +2329,22 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2015,7 +2358,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>117</v>
       </c>
@@ -2029,7 +2372,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>117</v>
       </c>
@@ -2043,7 +2386,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
         <v>117</v>
       </c>
@@ -2057,7 +2400,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>117</v>
       </c>
@@ -2071,7 +2414,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
         <v>117</v>
       </c>
@@ -2087,14 +2430,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="C5" r:id="rId3"/>
-    <hyperlink ref="B6" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="B4" r:id="rId6"/>
-    <hyperlink ref="A2" r:id="rId7" location="!/registration/login"/>
-    <hyperlink ref="A3:A6" r:id="rId8" location="!/registration/login" display="https://stg.imiassist.ai/agent/#!/registration/login"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
+    <hyperlink ref="B4" r:id="rId6" xr:uid="{00000000-0004-0000-0800-000005000000}"/>
+    <hyperlink ref="A2" r:id="rId7" location="!/registration/login" xr:uid="{00000000-0004-0000-0800-000006000000}"/>
+    <hyperlink ref="A3:A6" r:id="rId8" location="!/registration/login" display="https://stg.imiassist.ai/agent/#!/registration/login" xr:uid="{00000000-0004-0000-0800-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId9"/>

</xml_diff>

<commit_message>
Updates on 12th Oct
</commit_message>
<xml_diff>
--- a/TestData/IMIassist_Automation_TestData.xlsx
+++ b/TestData/IMIassist_Automation_TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IMI_Automation\IMI_Automation_files\Staging_IMIAssist_Automation\IMIAssist_Automtion\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IMI_Automation\IMIAssist_Automtion\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6646A7A-331A-4A73-A5A2-12625296C7BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="9" activeTab="13"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="15" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login_testdata" sheetId="1" r:id="rId1"/>
@@ -26,18 +27,30 @@
     <sheet name="Invalidusername" sheetId="5" r:id="rId12"/>
     <sheet name="Invalidpassword" sheetId="6" r:id="rId13"/>
     <sheet name="IMIA_Dashboard" sheetId="15" r:id="rId14"/>
+    <sheet name="AdminSettings_User" sheetId="16" r:id="rId15"/>
+    <sheet name="AdminSettings_Team" sheetId="17" r:id="rId16"/>
+    <sheet name="Team_PageDesign_AppLanding" sheetId="18" r:id="rId17"/>
+    <sheet name="Team_PageDesign_Onboarding" sheetId="19" r:id="rId18"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="203">
   <si>
     <t>URL</t>
   </si>
@@ -461,12 +474,198 @@
   </si>
   <si>
     <t>InvalidPassword</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Success_or_Error?</t>
+  </si>
+  <si>
+    <t>FirstName is Empty</t>
+  </si>
+  <si>
+    <t>Special chars in FirstName</t>
+  </si>
+  <si>
+    <t>Select Role Empty</t>
+  </si>
+  <si>
+    <t>Expected_Msg_FieldLevel</t>
+  </si>
+  <si>
+    <t>Expected_Msg_Header</t>
+  </si>
+  <si>
+    <t>TestType</t>
+  </si>
+  <si>
+    <t>Negative</t>
+  </si>
+  <si>
+    <t>Possitive</t>
+  </si>
+  <si>
+    <t>Ravi</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Specialty Admin</t>
+  </si>
+  <si>
+    <t>Bolla</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>r@v8</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Please Enter First Name</t>
+  </si>
+  <si>
+    <t>Empty Email</t>
+  </si>
+  <si>
+    <t>Please Enter Email</t>
+  </si>
+  <si>
+    <t>rav</t>
+  </si>
+  <si>
+    <t>Please select user's role</t>
+  </si>
+  <si>
+    <t>Please enter letters only</t>
+  </si>
+  <si>
+    <t>Successful Creation_User</t>
+  </si>
+  <si>
+    <t>Successful Creation_SpAdmin</t>
+  </si>
+  <si>
+    <t>User created successfully. Email sent to user with credentials.</t>
+  </si>
+  <si>
+    <t>Speciality</t>
+  </si>
+  <si>
+    <t>TeamName</t>
+  </si>
+  <si>
+    <t>Create New Team</t>
+  </si>
+  <si>
+    <t>Create New Team with existing data</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>A team already exists with the same name</t>
+  </si>
+  <si>
+    <t>MemberEmail</t>
+  </si>
+  <si>
+    <t>SelectRole</t>
+  </si>
+  <si>
+    <t>Add members to the team</t>
+  </si>
+  <si>
+    <t>Clinician</t>
+  </si>
+  <si>
+    <t>Successfully added user to the team</t>
+  </si>
+  <si>
+    <t>BrandColor</t>
+  </si>
+  <si>
+    <t>FontColor</t>
+  </si>
+  <si>
+    <t>Font</t>
+  </si>
+  <si>
+    <t>BrandLogo</t>
+  </si>
+  <si>
+    <t>AppTagline</t>
+  </si>
+  <si>
+    <t>AppDesc</t>
+  </si>
+  <si>
+    <t>ButtonColor</t>
+  </si>
+  <si>
+    <t>ButtonLabel</t>
+  </si>
+  <si>
+    <t>Successfully updated team page design</t>
+  </si>
+  <si>
+    <t>Page Design in App Landing</t>
+  </si>
+  <si>
+    <t>#dddd34</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Open Sans</t>
+  </si>
+  <si>
+    <t>Video Consultation</t>
+  </si>
+  <si>
+    <t>Get medical advice and assistance without the need to visit the hospital.</t>
+  </si>
+  <si>
+    <t>D:\IMI_Automation\IMIAssist_Automtion\TestData\NewLogo.jpeg</t>
+  </si>
+  <si>
+    <t>Proceed to Call.</t>
+  </si>
+  <si>
+    <t>Page Design Onboarding</t>
+  </si>
+  <si>
+    <t>tmsrafi.qa@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy&quot; &quot;hh&quot;:&quot;mm"/>
   </numFmts>
@@ -542,12 +741,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -563,7 +768,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
@@ -641,6 +846,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -955,21 +1161,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -980,7 +1186,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>117</v>
       </c>
@@ -993,8 +1199,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2" location="!/registration/login" display="https://stg.imiassist.ai/agent/ - !/registration/login"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId2" location="!/registration/login" display="https://stg.imiassist.ai/agent/ - !/registration/login" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -1002,23 +1208,23 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1035,7 +1241,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>117</v>
       </c>
@@ -1054,36 +1260,37 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="A2" r:id="rId4" location="!/registration/login"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
+    <hyperlink ref="A2" r:id="rId4" location="!/registration/login" xr:uid="{00000000-0004-0000-0900-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.54296875" customWidth="1"/>
-    <col min="5" max="5" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1112,7 +1319,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>117</v>
       </c>
@@ -1143,9 +1350,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2" location="!/registration/login"/>
-    <hyperlink ref="F2" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId2" location="!/registration/login" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId3" xr:uid="{00000000-0004-0000-0A00-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId4"/>
@@ -1153,21 +1360,21 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1178,7 +1385,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>117</v>
       </c>
@@ -1191,30 +1398,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="A2" r:id="rId3" location="!/registration/login"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0B00-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId3" location="!/registration/login" xr:uid="{00000000-0004-0000-0B00-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.26953125" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1225,7 +1433,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>117</v>
       </c>
@@ -1238,30 +1446,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2"/>
-    <hyperlink ref="A2" r:id="rId3" location="!/registration/login"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0C00-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0C00-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId3" location="!/registration/login" xr:uid="{00000000-0004-0000-0C00-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
         <v>19</v>
       </c>
@@ -1272,7 +1481,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>117</v>
       </c>
@@ -1285,32 +1494,523 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2" location="!/registration/login"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId2" location="!/registration/login" xr:uid="{00000000-0004-0000-0D00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E76F3CF-40A2-4FC7-97CF-E7F60422CA6B}">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E2" t="str">
+        <f ca="1">"Testinguser"&amp;TEXT(NOW(),"ddmm")&amp;"@gmail.com"</f>
+        <v>Testinguser1210@gmail.com</v>
+      </c>
+      <c r="G2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D3" t="s">
+        <v>155</v>
+      </c>
+      <c r="E3" t="str">
+        <f ca="1">"Testinguser"&amp;TEXT(NOW(),"ddmm")&amp;"@gmail.com"</f>
+        <v>Testinguser1210@gmail.com</v>
+      </c>
+      <c r="F3" t="s">
+        <v>156</v>
+      </c>
+      <c r="G3" t="s">
+        <v>161</v>
+      </c>
+      <c r="I3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D4" t="s">
+        <v>155</v>
+      </c>
+      <c r="E4" t="str">
+        <f ca="1">"Testinguser"&amp;TEXT(NOW(),"ddmm")&amp;"@gmail.com"</f>
+        <v>Testinguser1210@gmail.com</v>
+      </c>
+      <c r="F4" t="s">
+        <v>156</v>
+      </c>
+      <c r="G4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" t="s">
+        <v>154</v>
+      </c>
+      <c r="D5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F5" t="s">
+        <v>156</v>
+      </c>
+      <c r="G5" t="s">
+        <v>161</v>
+      </c>
+      <c r="I5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D6" t="s">
+        <v>155</v>
+      </c>
+      <c r="E6" t="s">
+        <v>166</v>
+      </c>
+      <c r="F6" t="s">
+        <v>156</v>
+      </c>
+      <c r="G6" t="s">
+        <v>161</v>
+      </c>
+      <c r="H6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B7" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D7" t="s">
+        <v>155</v>
+      </c>
+      <c r="E7" t="str">
+        <f ca="1">"Testinguser"&amp;TEXT(NOW(),"ddmm")&amp;"@gmail.com"</f>
+        <v>Testinguser1210@gmail.com</v>
+      </c>
+      <c r="F7" t="s">
+        <v>156</v>
+      </c>
+      <c r="G7" t="s">
+        <v>162</v>
+      </c>
+      <c r="I7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D8" t="s">
+        <v>159</v>
+      </c>
+      <c r="E8" t="str">
+        <f ca="1">"Testingspa"&amp;TEXT(NOW(),"ddmm")&amp;"@gmail.com"</f>
+        <v>Testingspa1210@gmail.com</v>
+      </c>
+      <c r="F8" t="s">
+        <v>157</v>
+      </c>
+      <c r="G8" t="s">
+        <v>162</v>
+      </c>
+      <c r="I8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB78D575-29B0-4222-9AD7-74A5DC55C0CF}">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D2" t="str">
+        <f ca="1">"TestTeam"&amp;TEXT(NOW()+4,"ddmm")</f>
+        <v>TestTeam1610</v>
+      </c>
+      <c r="F2" t="str">
+        <f ca="1">"Successfully created team : "&amp;D2</f>
+        <v>Successfully created team : TestTeam1610</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D3" t="str">
+        <f ca="1">"TestTeam"&amp;TEXT(NOW()+4,"ddmm")</f>
+        <v>TestTeam1610</v>
+      </c>
+      <c r="F3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C4" t="str">
+        <f>C2</f>
+        <v>Testing</v>
+      </c>
+      <c r="D4" t="str">
+        <f ca="1">D2</f>
+        <v>TestTeam1610</v>
+      </c>
+      <c r="F4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G4" t="s">
+        <v>202</v>
+      </c>
+      <c r="H4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G5" t="str">
+        <f ca="1">AdminSettings_User!E7</f>
+        <v>Testinguser1210@gmail.com</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1DACA2D-39CC-442D-B192-4F8F021A616A}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.140625" customWidth="1"/>
+    <col min="9" max="9" width="36.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>199</v>
+      </c>
+      <c r="G2" t="s">
+        <v>197</v>
+      </c>
+      <c r="H2" t="s">
+        <v>198</v>
+      </c>
+      <c r="I2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28AA50C2-D2F0-46A0-8CB0-E70CAB9D1561}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1327,7 +2027,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>117</v>
       </c>
@@ -1346,36 +2046,37 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="A2" r:id="rId4" location="!/registration/login" display="https://stg.imiassist.ai/agent/ - !/registration/login"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="A2" r:id="rId4" location="!/registration/login" display="https://stg.imiassist.ai/agent/ - !/registration/login" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="18.54296875" style="8" customWidth="1"/>
+    <col min="1" max="1" width="49.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="8" customWidth="1"/>
     <col min="5" max="5" width="22" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.1796875" style="8"/>
-    <col min="8" max="8" width="33.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="8"/>
+    <col min="6" max="7" width="9.140625" style="8"/>
+    <col min="8" max="8" width="33.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1404,7 +2105,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>117</v>
       </c>
@@ -1435,8 +2136,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2" location="!/registration/login" display="https://stg.imiassist.ai/agent/ - !/registration/login"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId2" location="!/registration/login" display="https://stg.imiassist.ai/agent/ - !/registration/login" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId3"/>
@@ -1444,39 +2145,39 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47" style="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.81640625" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.81640625" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.7265625" style="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.54296875" style="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.453125" style="27" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.453125" style="27" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7265625" style="27"/>
-    <col min="9" max="9" width="13.81640625" style="27" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.453125" style="27" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.1796875" style="27" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.81640625" style="27" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.453125" style="27" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.26953125" style="27" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.7265625" style="27" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.453125" style="27" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.26953125" style="27" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="35.08984375" style="27" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.81640625" style="27" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="26.08984375" style="27" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.7265625" style="27"/>
+    <col min="2" max="2" width="22.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="27"/>
+    <col min="9" max="9" width="13.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" style="27" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.7109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.28515625" style="27" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="35.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="26.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.7109375" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>19</v>
       </c>
@@ -1541,7 +2242,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="30" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" s="30" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>117</v>
       </c>
@@ -1580,7 +2281,7 @@
       </c>
       <c r="M2" s="32">
         <f ca="1">NOW()+3</f>
-        <v>44114.653952314817</v>
+        <v>44119.824964120373</v>
       </c>
       <c r="N2" s="30" t="s">
         <v>11</v>
@@ -1607,19 +2308,19 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B6" s="30" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="O2" r:id="rId4"/>
-    <hyperlink ref="J2" r:id="rId5"/>
-    <hyperlink ref="A2" r:id="rId6" location="!/registration/login"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="O2" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="J2" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="A2" r:id="rId6" location="!/registration/login" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId7"/>
@@ -1627,24 +2328,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="35">
         <f>DATE(2020,9,7)+1</f>
         <v>44082</v>
@@ -1652,39 +2353,40 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.453125" style="21" customWidth="1"/>
-    <col min="3" max="3" width="28.26953125" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.453125" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7265625" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" style="21"/>
-    <col min="7" max="7" width="25.1796875" style="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7265625" style="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.26953125" style="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.1796875" style="21"/>
-    <col min="11" max="11" width="22.26953125" style="21" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.453125" style="21" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.1796875" style="21"/>
-    <col min="14" max="14" width="23.453125" style="21" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="30.453125" style="21" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.453125" style="21" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.1796875" style="21"/>
+    <col min="1" max="1" width="14.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" style="21" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="21"/>
+    <col min="7" max="7" width="25.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="21"/>
+    <col min="11" max="11" width="22.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="21"/>
+    <col min="14" max="14" width="23.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>85</v>
       </c>
@@ -1734,7 +2436,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>86</v>
       </c>
@@ -1787,8 +2489,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="G2" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="G2" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -1796,21 +2498,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>120</v>
       </c>
@@ -1826,45 +2528,46 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1"/>
-    <hyperlink ref="D1" r:id="rId2"/>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="D1" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.26953125" style="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" style="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" style="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" style="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.453125" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.54296875" style="18" customWidth="1"/>
-    <col min="7" max="7" width="23.453125" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.81640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7265625" style="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.7265625" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.5703125" style="18" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.7109375" style="18" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" style="18" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.453125" style="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.54296875" style="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.453125" style="18" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.453125" style="18" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.1796875" style="18" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.1796875" style="19" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="42.54296875" style="18" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.1796875" style="18"/>
+    <col min="12" max="12" width="23.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="42.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="13" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" s="13" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>44</v>
       </c>
@@ -1923,7 +2626,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="15" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>52</v>
       </c>
@@ -1978,7 +2681,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
@@ -1986,22 +2689,22 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2015,7 +2718,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>117</v>
       </c>
@@ -2029,7 +2732,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>117</v>
       </c>
@@ -2043,7 +2746,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
         <v>117</v>
       </c>
@@ -2057,7 +2760,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>117</v>
       </c>
@@ -2071,7 +2774,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
         <v>117</v>
       </c>
@@ -2087,14 +2790,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="C5" r:id="rId3"/>
-    <hyperlink ref="B6" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="B4" r:id="rId6"/>
-    <hyperlink ref="A2" r:id="rId7" location="!/registration/login"/>
-    <hyperlink ref="A3:A6" r:id="rId8" location="!/registration/login" display="https://stg.imiassist.ai/agent/#!/registration/login"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
+    <hyperlink ref="B4" r:id="rId6" xr:uid="{00000000-0004-0000-0800-000005000000}"/>
+    <hyperlink ref="A2" r:id="rId7" location="!/registration/login" xr:uid="{00000000-0004-0000-0800-000006000000}"/>
+    <hyperlink ref="A3:A6" r:id="rId8" location="!/registration/login" display="https://stg.imiassist.ai/agent/#!/registration/login" xr:uid="{00000000-0004-0000-0800-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId9"/>

</xml_diff>

<commit_message>
Created Cases module cases folder
</commit_message>
<xml_diff>
--- a/TestData/IMIassist_Automation_TestData.xlsx
+++ b/TestData/IMIassist_Automation_TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15530" windowHeight="8300" firstSheet="9" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15530" windowHeight="8300" firstSheet="9" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Login_testdata" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="Invalidusername" sheetId="5" r:id="rId12"/>
     <sheet name="Invalidpassword" sheetId="6" r:id="rId13"/>
     <sheet name="IMIA_Dashboard" sheetId="15" r:id="rId14"/>
+    <sheet name="IMIA_Cases" sheetId="16" r:id="rId15"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="145">
   <si>
     <t>URL</t>
   </si>
@@ -467,6 +468,12 @@
   </si>
   <si>
     <t>https://preprod.imiassist.ai/agent/#!/registration/login</t>
+  </si>
+  <si>
+    <t>Case_ID</t>
+  </si>
+  <si>
+    <t>test-863</t>
   </si>
 </sst>
 </file>
@@ -1011,7 +1018,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1254,10 +1261,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1290,29 +1297,49 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="28"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="29"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A3" t="s">
         <v>142</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B3" t="s">
         <v>141</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C3" s="29" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId1"/>
     <hyperlink ref="C2" r:id="rId2"/>
     <hyperlink ref="A2" r:id="rId3" location="!/registration/login"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1603,7 +1630,7 @@
       </c>
       <c r="M2" s="32">
         <f ca="1">NOW()+3</f>
-        <v>44116.703673958335</v>
+        <v>44119.895683564813</v>
       </c>
       <c r="N2" s="30" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Added case's module test case's
</commit_message>
<xml_diff>
--- a/TestData/IMIassist_Automation_TestData.xlsx
+++ b/TestData/IMIassist_Automation_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IMI_Automation\IMIAssist_Automtion\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="209">
   <si>
     <t>URL</t>
   </si>
@@ -480,9 +480,6 @@
     <t>Case_ID</t>
   </si>
   <si>
-    <t>test-863</t>
-  </si>
-  <si>
     <t>TestType</t>
   </si>
   <si>
@@ -667,6 +664,15 @@
   </si>
   <si>
     <t>Proceed to Call.</t>
+  </si>
+  <si>
+    <t>Historyoptiontext</t>
+  </si>
+  <si>
+    <t>Chat History</t>
+  </si>
+  <si>
+    <t>test-879</t>
   </si>
 </sst>
 </file>
@@ -1573,22 +1579,28 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>144</v>
+        <v>208</v>
+      </c>
+      <c r="B2" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -1622,126 +1634,126 @@
         <v>70</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>151</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" t="s">
         <v>153</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>154</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>155</v>
-      </c>
-      <c r="D2" t="s">
-        <v>156</v>
       </c>
       <c r="E2" t="str">
         <f ca="1">"Testinguser"&amp;TEXT(NOW(),"ddmm")&amp;"@gmail.com"</f>
-        <v>Testinguser1210@gmail.com</v>
+        <v>Testinguser1410@gmail.com</v>
       </c>
       <c r="G2" t="s">
+        <v>156</v>
+      </c>
+      <c r="I2" t="s">
         <v>157</v>
-      </c>
-      <c r="I2" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E3" t="str">
         <f ca="1">"Testinguser"&amp;TEXT(NOW(),"ddmm")&amp;"@gmail.com"</f>
-        <v>Testinguser1210@gmail.com</v>
+        <v>Testinguser1410@gmail.com</v>
       </c>
       <c r="F3" t="s">
+        <v>159</v>
+      </c>
+      <c r="G3" t="s">
+        <v>156</v>
+      </c>
+      <c r="I3" t="s">
         <v>160</v>
-      </c>
-      <c r="G3" t="s">
-        <v>157</v>
-      </c>
-      <c r="I3" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C4" t="s">
         <v>162</v>
       </c>
-      <c r="B4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C4" t="s">
-        <v>163</v>
-      </c>
       <c r="D4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E4" t="str">
         <f ca="1">"Testinguser"&amp;TEXT(NOW(),"ddmm")&amp;"@gmail.com"</f>
-        <v>Testinguser1210@gmail.com</v>
+        <v>Testinguser1410@gmail.com</v>
       </c>
       <c r="F4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C5" t="s">
+        <v>154</v>
+      </c>
+      <c r="D5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F5" t="s">
+        <v>159</v>
+      </c>
+      <c r="G5" t="s">
+        <v>156</v>
+      </c>
+      <c r="I5" t="s">
         <v>165</v>
-      </c>
-      <c r="B5" t="s">
-        <v>154</v>
-      </c>
-      <c r="C5" t="s">
-        <v>155</v>
-      </c>
-      <c r="D5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F5" t="s">
-        <v>160</v>
-      </c>
-      <c r="G5" t="s">
-        <v>157</v>
-      </c>
-      <c r="I5" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -1749,22 +1761,22 @@
         <v>136</v>
       </c>
       <c r="B6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C6" t="s">
         <v>154</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>155</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
+        <v>166</v>
+      </c>
+      <c r="F6" t="s">
+        <v>159</v>
+      </c>
+      <c r="G6" t="s">
         <v>156</v>
-      </c>
-      <c r="E6" t="s">
-        <v>167</v>
-      </c>
-      <c r="F6" t="s">
-        <v>160</v>
-      </c>
-      <c r="G6" t="s">
-        <v>157</v>
       </c>
       <c r="H6" t="s">
         <v>136</v>
@@ -1772,56 +1784,56 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>167</v>
+      </c>
+      <c r="B7" t="s">
         <v>168</v>
       </c>
-      <c r="B7" t="s">
-        <v>169</v>
-      </c>
       <c r="C7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D7" t="s">
         <v>155</v>
-      </c>
-      <c r="D7" t="s">
-        <v>156</v>
       </c>
       <c r="E7" t="str">
         <f ca="1">"Testinguser"&amp;TEXT(NOW(),"ddmm")&amp;"@gmail.com"</f>
-        <v>Testinguser1210@gmail.com</v>
+        <v>Testinguser1410@gmail.com</v>
       </c>
       <c r="F7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G7" t="s">
+        <v>169</v>
+      </c>
+      <c r="I7" t="s">
         <v>170</v>
-      </c>
-      <c r="I7" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C8" t="s">
         <v>172</v>
       </c>
-      <c r="B8" t="s">
-        <v>169</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>173</v>
-      </c>
-      <c r="D8" t="s">
-        <v>174</v>
       </c>
       <c r="E8" t="str">
         <f ca="1">"Testingspa"&amp;TEXT(NOW(),"ddmm")&amp;"@gmail.com"</f>
-        <v>Testingspa1210@gmail.com</v>
+        <v>Testingspa1410@gmail.com</v>
       </c>
       <c r="F8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G8" t="s">
+        <v>169</v>
+      </c>
+      <c r="I8" t="s">
         <v>170</v>
-      </c>
-      <c r="I8" t="s">
-        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -1854,70 +1866,70 @@
         <v>70</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>178</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B2" t="s">
         <v>180</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>181</v>
-      </c>
-      <c r="C2" t="s">
-        <v>182</v>
       </c>
       <c r="D2" t="str">
         <f ca="1">"TestTeam"&amp;TEXT(NOW()+4,"ddmm")</f>
-        <v>TestTeam1610</v>
+        <v>TestTeam1810</v>
       </c>
       <c r="F2" t="str">
         <f ca="1">"Successfully created team : "&amp;D2</f>
-        <v>Successfully created team : TestTeam1610</v>
+        <v>Successfully created team : TestTeam1810</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D3" t="str">
         <f ca="1">"TestTeam"&amp;TEXT(NOW()+4,"ddmm")</f>
-        <v>TestTeam1610</v>
+        <v>TestTeam1810</v>
       </c>
       <c r="F3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C4" t="str">
         <f>C2</f>
@@ -1925,21 +1937,21 @@
       </c>
       <c r="D4" t="str">
         <f ca="1">D2</f>
-        <v>TestTeam1610</v>
+        <v>TestTeam1810</v>
       </c>
       <c r="F4" t="s">
+        <v>185</v>
+      </c>
+      <c r="G4" t="s">
         <v>186</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>187</v>
-      </c>
-      <c r="H4" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G5" t="str">
-        <f ca="1">[1]AdminSettings_User!E7</f>
+        <f>[1]AdminSettings_User!E7</f>
         <v>Testinguser1210@gmail.com</v>
       </c>
     </row>
@@ -1970,57 +1982,57 @@
         <v>70</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>194</v>
-      </c>
       <c r="I1" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C2" t="s">
         <v>195</v>
       </c>
-      <c r="B2" t="s">
-        <v>181</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>196</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>197</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="39" t="s">
         <v>198</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="G2" t="s">
         <v>199</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>200</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>201</v>
-      </c>
-      <c r="I2" t="s">
-        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -2050,33 +2062,33 @@
         <v>70</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>204</v>
-      </c>
       <c r="E1" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" t="s">
         <v>205</v>
       </c>
-      <c r="B2" t="s">
-        <v>181</v>
-      </c>
-      <c r="C2" t="s">
-        <v>196</v>
-      </c>
-      <c r="D2" t="s">
-        <v>206</v>
-      </c>
       <c r="E2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -2371,7 +2383,7 @@
       </c>
       <c r="M2" s="32">
         <f ca="1">NOW()+3</f>
-        <v>44119.902088194445</v>
+        <v>44121.735168055558</v>
       </c>
       <c r="N2" s="30" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Committed with Completed cases
</commit_message>
<xml_diff>
--- a/TestData/IMIassist_Automation_TestData.xlsx
+++ b/TestData/IMIassist_Automation_TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IMI_Automation\IMIAssist_Automtion\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8D2379-BEB7-4958-8968-5C6175991122}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="14" activeTab="14"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login_testdata" sheetId="1" r:id="rId1"/>
@@ -31,21 +32,106 @@
     <sheet name="AdminSettings_Team" sheetId="18" r:id="rId17"/>
     <sheet name="Team_PageDesign_AppLanding" sheetId="19" r:id="rId18"/>
     <sheet name="Team_PageDesign_Onboarding" sheetId="21" r:id="rId19"/>
+    <sheet name="Team_PageDesign_VideoCall" sheetId="22" r:id="rId20"/>
+    <sheet name="Team_PageDesign_LinkExpiry" sheetId="23" r:id="rId21"/>
+    <sheet name="Team_Settings_General" sheetId="24" r:id="rId22"/>
+    <sheet name="Team_Settings_Notification" sheetId="25" r:id="rId23"/>
+    <sheet name="Team_Settings_Feedback" sheetId="26" r:id="rId24"/>
+    <sheet name="Team_Theme_Settings" sheetId="27" r:id="rId25"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId20"/>
+    <externalReference r:id="rId26"/>
   </externalReferences>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Ravi Bolla</author>
+  </authors>
+  <commentList>
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{C32ABAA7-0266-48E3-AB60-9EF366F076CC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ravi Bolla:
+SelectByValue</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+UK (  +00:00 / +01:00 )</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Ravi Bolla</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{BBE218CF-3A3A-443B-8453-792ED958AC3B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ravi Bolla:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Fill Input1,inpu2,input 3 incase 'Multiple choice'
+Comment_Description in case of 'Comment Question'
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="278">
   <si>
     <t>URL</t>
   </si>
@@ -633,9 +719,6 @@
     <t>AppDesc</t>
   </si>
   <si>
-    <t>Page Design in App Landing</t>
-  </si>
-  <si>
     <t>#dddd34</t>
   </si>
   <si>
@@ -663,20 +746,236 @@
     <t>ButtonLabel</t>
   </si>
   <si>
-    <t>Page Design Onboarding</t>
-  </si>
-  <si>
     <t>Proceed to Call.</t>
+  </si>
+  <si>
+    <t>SupportPerson</t>
+  </si>
+  <si>
+    <t>VideoOnFocus</t>
+  </si>
+  <si>
+    <t>PatientQA</t>
+  </si>
+  <si>
+    <t>Page Design: Lnik Expiry</t>
+  </si>
+  <si>
+    <t>Page Design: Video call interface</t>
+  </si>
+  <si>
+    <t>Page Design: Onboarding</t>
+  </si>
+  <si>
+    <t>Page Design: App Landing</t>
+  </si>
+  <si>
+    <t>The appointment has expired. Please close the window and contact customer support for further assistance.</t>
+  </si>
+  <si>
+    <t>LE_Description</t>
+  </si>
+  <si>
+    <t>Team Settings: General</t>
+  </si>
+  <si>
+    <t>TimeZone</t>
+  </si>
+  <si>
+    <t>DefaultCountryCode</t>
+  </si>
+  <si>
+    <t>Episode_Archiving</t>
+  </si>
+  <si>
+    <t>Episode_GeoLocation</t>
+  </si>
+  <si>
+    <t>Team Settings: Notification</t>
+  </si>
+  <si>
+    <t>EmailHeader</t>
+  </si>
+  <si>
+    <t>EmailFooter</t>
+  </si>
+  <si>
+    <t>SenderEmail</t>
+  </si>
+  <si>
+    <t>SubjectLine</t>
+  </si>
+  <si>
+    <t>EmailBody</t>
+  </si>
+  <si>
+    <t>SMStemp_Body</t>
+  </si>
+  <si>
+    <t>Team Settings: Feedback</t>
+  </si>
+  <si>
+    <t>Question2</t>
+  </si>
+  <si>
+    <t>QuestionType</t>
+  </si>
+  <si>
+    <t>Input1</t>
+  </si>
+  <si>
+    <t>Input2</t>
+  </si>
+  <si>
+    <t>Input3</t>
+  </si>
+  <si>
+    <t>Comment_Description</t>
+  </si>
+  <si>
+    <t>United Kingdom +44</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>D:\IMI_Automation\IMIAssist_Automtion\TestData\Header.jpeg</t>
+  </si>
+  <si>
+    <t>D:\IMI_Automation\IMIAssist_Automtion\TestData\Footer.jpeg</t>
+  </si>
+  <si>
+    <t>noreply@eclinic.org.uk</t>
+  </si>
+  <si>
+    <t>Your upcoming video appointment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Based on your query, our clinician has invited you to join in for a video consultation session. Please click on the link to connect to agent. If you're an android user, use Chrome browser and if you're an iOS user use Safari(v11 &amp; above). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use the following link to start a video consultation with our clinician. For Android use Chrome and for IOS use Safari (11+) </t>
+  </si>
+  <si>
+    <t>Successfully updated notification settings</t>
+  </si>
+  <si>
+    <t>Successfully updated general settings.</t>
+  </si>
+  <si>
+    <t>Your overall feedback</t>
+  </si>
+  <si>
+    <t>Question successfully added.</t>
+  </si>
+  <si>
+    <t>Multiple choice</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Not Sure</t>
+  </si>
+  <si>
+    <t>Europe/London</t>
+  </si>
+  <si>
+    <t>Comment question</t>
+  </si>
+  <si>
+    <t>PageFont</t>
+  </si>
+  <si>
+    <t>FontColour</t>
+  </si>
+  <si>
+    <t>AddressAgentBy</t>
+  </si>
+  <si>
+    <t>AddressCustomerBy</t>
+  </si>
+  <si>
+    <t>ClinicianQA</t>
+  </si>
+  <si>
+    <t>D:\IMI_Automation\IMIAssist_Automtion\TestData\BrandLogo.jpeg</t>
+  </si>
+  <si>
+    <t>Theme Settings: change</t>
+  </si>
+  <si>
+    <t>Theme Settings: original</t>
+  </si>
+  <si>
+    <t>Arial</t>
+  </si>
+  <si>
+    <t>Successfully updated Specialty Settings</t>
+  </si>
+  <si>
+    <t>BrandColour_Code</t>
+  </si>
+  <si>
+    <t>ButtonColor_Code</t>
+  </si>
+  <si>
+    <t>rgb(34, 64, 0)</t>
+  </si>
+  <si>
+    <t>rgb(128, 128, 128)</t>
+  </si>
+  <si>
+    <t>rgb(18, 52, 86)</t>
+  </si>
+  <si>
+    <t>rgb(84, 84, 84)</t>
+  </si>
+  <si>
+    <t>#123456</t>
+  </si>
+  <si>
+    <t>#545454</t>
+  </si>
+  <si>
+    <t>WHITE</t>
+  </si>
+  <si>
+    <t>D:\IMI_Automation\IMIAssist_Automtion\TestData\logoInv</t>
+  </si>
+  <si>
+    <t>D:\IMI_Automation\IMIAssist_Automtion\TestData\LogoMore2MB.jpg</t>
+  </si>
+  <si>
+    <t>D:\IMI_Automation\IMIAssist_Automtion\TestData\logo2.png</t>
+  </si>
+  <si>
+    <t>#808080</t>
+  </si>
+  <si>
+    <t>File size is greater than 2MB</t>
+  </si>
+  <si>
+    <t>Upload image file. Only PNG, JPG , JPEG are allowed</t>
+  </si>
+  <si>
+    <t>holmojipsu@nedoz.com</t>
+  </si>
+  <si>
+    <t>Assist5678</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy&quot; &quot;hh&quot;:&quot;mm"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -746,6 +1045,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1221,21 +1533,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1246,7 +1558,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>117</v>
       </c>
@@ -1257,34 +1569,46 @@
         <v>4</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" t="s">
+        <v>276</v>
+      </c>
+      <c r="C3" t="s">
+        <v>277</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2" location="!/registration/login" display="https://stg.imiassist.ai/agent/ - !/registration/login"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId2" location="!/registration/login" display="https://stg.imiassist.ai/agent/ - !/registration/login" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A3" r:id="rId3" location="!/registration/login" xr:uid="{A0694443-C55E-47ED-BEEB-809F1C26D7A8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1301,7 +1625,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>117</v>
       </c>
@@ -1320,36 +1644,37 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="A2" r:id="rId4" location="!/registration/login"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
+    <hyperlink ref="A2" r:id="rId4" location="!/registration/login" xr:uid="{00000000-0004-0000-0900-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.54296875" customWidth="1"/>
-    <col min="5" max="5" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1378,7 +1703,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>117</v>
       </c>
@@ -1409,9 +1734,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2" location="!/registration/login"/>
-    <hyperlink ref="F2" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId2" location="!/registration/login" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId3" xr:uid="{00000000-0004-0000-0A00-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId4"/>
@@ -1419,21 +1744,21 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1444,7 +1769,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>117</v>
       </c>
@@ -1457,30 +1782,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="A2" r:id="rId3" location="!/registration/login"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0B00-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId3" location="!/registration/login" xr:uid="{00000000-0004-0000-0B00-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.26953125" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1491,7 +1817,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>117</v>
       </c>
@@ -1504,30 +1830,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2"/>
-    <hyperlink ref="A2" r:id="rId3" location="!/registration/login"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0C00-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0C00-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId3" location="!/registration/login" xr:uid="{00000000-0004-0000-0C00-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
         <v>19</v>
       </c>
@@ -1538,7 +1865,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>117</v>
       </c>
@@ -1549,7 +1876,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>142</v>
       </c>
@@ -1562,9 +1889,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2"/>
-    <hyperlink ref="A2" r:id="rId3" location="!/registration/login"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0D00-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId3" location="!/registration/login" xr:uid="{00000000-0004-0000-0D00-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
@@ -1572,52 +1899,53 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>144</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.81640625" customWidth="1"/>
-    <col min="2" max="2" width="17.81640625" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" customWidth="1"/>
-    <col min="4" max="4" width="13.81640625" customWidth="1"/>
-    <col min="5" max="5" width="28.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7265625" customWidth="1"/>
-    <col min="7" max="7" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.54296875" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>70</v>
       </c>
@@ -1646,7 +1974,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>153</v>
       </c>
@@ -1661,7 +1989,7 @@
       </c>
       <c r="E2" t="str">
         <f ca="1">"Testinguser"&amp;TEXT(NOW(),"ddmm")&amp;"@gmail.com"</f>
-        <v>Testinguser1210@gmail.com</v>
+        <v>Testinguser1510@gmail.com</v>
       </c>
       <c r="G2" t="s">
         <v>157</v>
@@ -1670,7 +1998,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>159</v>
       </c>
@@ -1682,7 +2010,7 @@
       </c>
       <c r="E3" t="str">
         <f ca="1">"Testinguser"&amp;TEXT(NOW(),"ddmm")&amp;"@gmail.com"</f>
-        <v>Testinguser1210@gmail.com</v>
+        <v>Testinguser1510@gmail.com</v>
       </c>
       <c r="F3" t="s">
         <v>160</v>
@@ -1694,7 +2022,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>162</v>
       </c>
@@ -1709,7 +2037,7 @@
       </c>
       <c r="E4" t="str">
         <f ca="1">"Testinguser"&amp;TEXT(NOW(),"ddmm")&amp;"@gmail.com"</f>
-        <v>Testinguser1210@gmail.com</v>
+        <v>Testinguser1510@gmail.com</v>
       </c>
       <c r="F4" t="s">
         <v>160</v>
@@ -1721,7 +2049,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>165</v>
       </c>
@@ -1744,7 +2072,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>136</v>
       </c>
@@ -1770,7 +2098,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>168</v>
       </c>
@@ -1785,7 +2113,7 @@
       </c>
       <c r="E7" t="str">
         <f ca="1">"Testinguser"&amp;TEXT(NOW(),"ddmm")&amp;"@gmail.com"</f>
-        <v>Testinguser1210@gmail.com</v>
+        <v>Testinguser1510@gmail.com</v>
       </c>
       <c r="F7" t="s">
         <v>160</v>
@@ -1797,7 +2125,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>172</v>
       </c>
@@ -1812,7 +2140,7 @@
       </c>
       <c r="E8" t="str">
         <f ca="1">"Testingspa"&amp;TEXT(NOW(),"ddmm")&amp;"@gmail.com"</f>
-        <v>Testingspa1210@gmail.com</v>
+        <v>Testingspa1510@gmail.com</v>
       </c>
       <c r="F8" t="s">
         <v>175</v>
@@ -1826,30 +2154,31 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" customWidth="1"/>
-    <col min="3" max="3" width="15.26953125" customWidth="1"/>
-    <col min="4" max="4" width="26.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>70</v>
       </c>
@@ -1875,7 +2204,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>180</v>
       </c>
@@ -1887,14 +2216,14 @@
       </c>
       <c r="D2" t="str">
         <f ca="1">"TestTeam"&amp;TEXT(NOW()+4,"ddmm")</f>
-        <v>TestTeam1610</v>
+        <v>TestTeam1910</v>
       </c>
       <c r="F2" t="str">
         <f ca="1">"Successfully created team : "&amp;D2</f>
-        <v>Successfully created team : TestTeam1610</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <v>Successfully created team : TestTeam1910</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>183</v>
       </c>
@@ -1906,13 +2235,13 @@
       </c>
       <c r="D3" t="str">
         <f ca="1">"TestTeam"&amp;TEXT(NOW()+4,"ddmm")</f>
-        <v>TestTeam1610</v>
+        <v>TestTeam1910</v>
       </c>
       <c r="F3" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>185</v>
       </c>
@@ -1925,7 +2254,7 @@
       </c>
       <c r="D4" t="str">
         <f ca="1">D2</f>
-        <v>TestTeam1610</v>
+        <v>TestTeam1910</v>
       </c>
       <c r="F4" t="s">
         <v>186</v>
@@ -1937,35 +2266,36 @@
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G5" t="str">
-        <f ca="1">[1]AdminSettings_User!E7</f>
+        <f>[1]AdminSettings_User!E7</f>
         <v>Testinguser1210@gmail.com</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.1796875" customWidth="1"/>
-    <col min="7" max="7" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.1796875" customWidth="1"/>
-    <col min="9" max="9" width="36.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.140625" customWidth="1"/>
+    <col min="9" max="9" width="36.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>70</v>
       </c>
@@ -1994,114 +2324,116 @@
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
       <c r="B2" t="s">
         <v>181</v>
       </c>
       <c r="C2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" t="s">
         <v>196</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>197</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="39" t="s">
         <v>198</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="G2" t="s">
         <v>199</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>200</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>201</v>
-      </c>
-      <c r="I2" t="s">
-        <v>202</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.453125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>205</v>
-      </c>
-      <c r="B2" t="s">
-        <v>181</v>
-      </c>
-      <c r="C2" t="s">
-        <v>196</v>
-      </c>
-      <c r="D2" t="s">
-        <v>206</v>
-      </c>
-      <c r="E2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2118,7 +2450,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>117</v>
       </c>
@@ -2137,36 +2469,618 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="A2" r:id="rId4" location="!/registration/login" display="https://stg.imiassist.ai/agent/ - !/registration/login"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="A2" r:id="rId4" location="!/registration/login" display="https://stg.imiassist.ai/agent/ - !/registration/login" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F118E3B-CAE8-48A4-BECA-93BBFCA72E5A}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FC6D7AD-BD40-443E-B761-3B1A9B4B24D9}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94FD6D2F-A727-4812-9E8E-C3407252748A}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="5" width="19.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2" t="s">
+        <v>249</v>
+      </c>
+      <c r="D2" t="s">
+        <v>233</v>
+      </c>
+      <c r="E2" t="s">
+        <v>234</v>
+      </c>
+      <c r="F2" t="s">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C05B4F3-465B-4BC5-8142-97003DE204EC}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>235</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>236</v>
+      </c>
+      <c r="E2" t="s">
+        <v>237</v>
+      </c>
+      <c r="F2" t="s">
+        <v>238</v>
+      </c>
+      <c r="G2" t="s">
+        <v>239</v>
+      </c>
+      <c r="H2" t="s">
+        <v>240</v>
+      </c>
+      <c r="I2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA6B764A-62B4-4DBF-931C-E54BF7A08AC8}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2" t="s">
+        <v>243</v>
+      </c>
+      <c r="D2" t="s">
+        <v>245</v>
+      </c>
+      <c r="E2" t="s">
+        <v>246</v>
+      </c>
+      <c r="F2" t="s">
+        <v>247</v>
+      </c>
+      <c r="G2" t="s">
+        <v>248</v>
+      </c>
+      <c r="I2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>250</v>
+      </c>
+      <c r="H3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A87FD931-04AB-4A7D-AF4C-3691A38D150A}">
+  <dimension ref="A1:M5"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="36.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>270</v>
+      </c>
+      <c r="D2" t="s">
+        <v>267</v>
+      </c>
+      <c r="E2" t="s">
+        <v>265</v>
+      </c>
+      <c r="F2" t="s">
+        <v>268</v>
+      </c>
+      <c r="G2" t="s">
+        <v>266</v>
+      </c>
+      <c r="H2" t="s">
+        <v>197</v>
+      </c>
+      <c r="I2" t="s">
+        <v>269</v>
+      </c>
+      <c r="J2" t="s">
+        <v>255</v>
+      </c>
+      <c r="K2" t="s">
+        <v>207</v>
+      </c>
+      <c r="L2" t="s">
+        <v>275</v>
+      </c>
+      <c r="M2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>271</v>
+      </c>
+      <c r="D3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E3" t="s">
+        <v>265</v>
+      </c>
+      <c r="F3" t="s">
+        <v>268</v>
+      </c>
+      <c r="G3" t="s">
+        <v>266</v>
+      </c>
+      <c r="H3" t="s">
+        <v>197</v>
+      </c>
+      <c r="I3" t="s">
+        <v>269</v>
+      </c>
+      <c r="J3" t="s">
+        <v>255</v>
+      </c>
+      <c r="K3" t="s">
+        <v>207</v>
+      </c>
+      <c r="L3" t="s">
+        <v>274</v>
+      </c>
+      <c r="M3" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>272</v>
+      </c>
+      <c r="D4" t="s">
+        <v>267</v>
+      </c>
+      <c r="E4" t="s">
+        <v>265</v>
+      </c>
+      <c r="F4" t="s">
+        <v>268</v>
+      </c>
+      <c r="G4" t="s">
+        <v>266</v>
+      </c>
+      <c r="H4" t="s">
+        <v>197</v>
+      </c>
+      <c r="I4" t="s">
+        <v>269</v>
+      </c>
+      <c r="J4" t="s">
+        <v>255</v>
+      </c>
+      <c r="K4" t="s">
+        <v>207</v>
+      </c>
+      <c r="M4" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>258</v>
+      </c>
+      <c r="B5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>256</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>263</v>
+      </c>
+      <c r="F5" t="s">
+        <v>273</v>
+      </c>
+      <c r="G5" t="s">
+        <v>264</v>
+      </c>
+      <c r="H5" t="s">
+        <v>259</v>
+      </c>
+      <c r="I5" t="s">
+        <v>269</v>
+      </c>
+      <c r="J5" t="s">
+        <v>255</v>
+      </c>
+      <c r="K5" t="s">
+        <v>207</v>
+      </c>
+      <c r="M5" t="s">
+        <v>260</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="18.54296875" style="8" customWidth="1"/>
+    <col min="1" max="1" width="49.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="8" customWidth="1"/>
     <col min="5" max="5" width="22" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.1796875" style="8"/>
-    <col min="8" max="8" width="33.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="8"/>
+    <col min="6" max="7" width="9.140625" style="8"/>
+    <col min="8" max="8" width="33.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2195,7 +3109,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>117</v>
       </c>
@@ -2226,8 +3140,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2" location="!/registration/login" display="https://stg.imiassist.ai/agent/ - !/registration/login"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId2" location="!/registration/login" display="https://stg.imiassist.ai/agent/ - !/registration/login" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId3"/>
@@ -2235,39 +3149,39 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47" style="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.81640625" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.81640625" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.7265625" style="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.54296875" style="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.453125" style="27" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.453125" style="27" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7265625" style="27"/>
-    <col min="9" max="9" width="13.81640625" style="27" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.453125" style="27" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.1796875" style="27" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.81640625" style="27" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.453125" style="27" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.26953125" style="27" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.7265625" style="27" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.453125" style="27" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.26953125" style="27" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="35.08984375" style="27" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.81640625" style="27" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="26.08984375" style="27" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.7265625" style="27"/>
+    <col min="2" max="2" width="22.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="27"/>
+    <col min="9" max="9" width="13.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" style="27" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.7109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.28515625" style="27" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="35.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="26.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.7109375" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>19</v>
       </c>
@@ -2332,7 +3246,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="30" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" s="30" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>117</v>
       </c>
@@ -2371,7 +3285,7 @@
       </c>
       <c r="M2" s="32">
         <f ca="1">NOW()+3</f>
-        <v>44119.902088194445</v>
+        <v>44122.844770717595</v>
       </c>
       <c r="N2" s="30" t="s">
         <v>11</v>
@@ -2398,19 +3312,19 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B6" s="30" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="O2" r:id="rId4"/>
-    <hyperlink ref="J2" r:id="rId5"/>
-    <hyperlink ref="A2" r:id="rId6" location="!/registration/login"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="O2" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="J2" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="A2" r:id="rId6" location="!/registration/login" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId7"/>
@@ -2418,24 +3332,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="35">
         <f>DATE(2020,9,7)+1</f>
         <v>44082</v>
@@ -2443,39 +3357,40 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.453125" style="21" customWidth="1"/>
-    <col min="3" max="3" width="28.26953125" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.453125" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7265625" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" style="21"/>
-    <col min="7" max="7" width="25.1796875" style="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7265625" style="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.26953125" style="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.1796875" style="21"/>
-    <col min="11" max="11" width="22.26953125" style="21" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.453125" style="21" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.1796875" style="21"/>
-    <col min="14" max="14" width="23.453125" style="21" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="30.453125" style="21" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.453125" style="21" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.1796875" style="21"/>
+    <col min="1" max="1" width="14.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" style="21" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="21"/>
+    <col min="7" max="7" width="25.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="21"/>
+    <col min="11" max="11" width="22.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="21"/>
+    <col min="14" max="14" width="23.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>85</v>
       </c>
@@ -2525,7 +3440,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>86</v>
       </c>
@@ -2578,8 +3493,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="G2" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="G2" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -2587,21 +3502,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>120</v>
       </c>
@@ -2617,45 +3532,46 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1"/>
-    <hyperlink ref="D1" r:id="rId2"/>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="D1" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.26953125" style="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" style="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" style="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" style="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.453125" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.54296875" style="18" customWidth="1"/>
-    <col min="7" max="7" width="23.453125" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.81640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7265625" style="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.7265625" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.5703125" style="18" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.7109375" style="18" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" style="18" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.453125" style="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.54296875" style="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.453125" style="18" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.453125" style="18" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.1796875" style="18" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.1796875" style="19" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="42.54296875" style="18" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.1796875" style="18"/>
+    <col min="12" max="12" width="23.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="42.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="13" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" s="13" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>44</v>
       </c>
@@ -2714,7 +3630,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="15" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>52</v>
       </c>
@@ -2769,7 +3685,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
@@ -2777,22 +3693,22 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2806,7 +3722,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>117</v>
       </c>
@@ -2820,7 +3736,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>117</v>
       </c>
@@ -2834,7 +3750,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
         <v>117</v>
       </c>
@@ -2848,7 +3764,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>117</v>
       </c>
@@ -2862,7 +3778,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
         <v>117</v>
       </c>
@@ -2878,14 +3794,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="C5" r:id="rId3"/>
-    <hyperlink ref="B6" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="B4" r:id="rId6"/>
-    <hyperlink ref="A2" r:id="rId7" location="!/registration/login"/>
-    <hyperlink ref="A3:A6" r:id="rId8" location="!/registration/login" display="https://stg.imiassist.ai/agent/#!/registration/login"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
+    <hyperlink ref="B4" r:id="rId6" xr:uid="{00000000-0004-0000-0800-000005000000}"/>
+    <hyperlink ref="A2" r:id="rId7" location="!/registration/login" xr:uid="{00000000-0004-0000-0800-000006000000}"/>
+    <hyperlink ref="A3:A6" r:id="rId8" location="!/registration/login" display="https://stg.imiassist.ai/agent/#!/registration/login" xr:uid="{00000000-0004-0000-0800-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId9"/>

</xml_diff>

<commit_message>
Added Create custom report test cases as part of sprint 33
</commit_message>
<xml_diff>
--- a/TestData/IMIassist_Automation_TestData.xlsx
+++ b/TestData/IMIassist_Automation_TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="14" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="19" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Login_testdata" sheetId="1" r:id="rId1"/>
@@ -32,9 +32,10 @@
     <sheet name="AdminSettings_Team" sheetId="18" r:id="rId18"/>
     <sheet name="Team_PageDesign_AppLanding" sheetId="19" r:id="rId19"/>
     <sheet name="Team_PageDesign_Onboarding" sheetId="21" r:id="rId20"/>
+    <sheet name="IMI_Custom_Reports" sheetId="23" r:id="rId21"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId21"/>
+    <externalReference r:id="rId22"/>
   </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="246">
   <si>
     <t>URL</t>
   </si>
@@ -748,14 +749,54 @@
   </si>
   <si>
     <t>CAPassword</t>
+  </si>
+  <si>
+    <t>riknuvufyo@nedoz.com</t>
+  </si>
+  <si>
+    <t>Team Admin</t>
+  </si>
+  <si>
+    <t>https://tempail.com/u/13/riknuvufyo-6313c3ab81/</t>
+  </si>
+  <si>
+    <t>TeamAdminUsername</t>
+  </si>
+  <si>
+    <t>Teamadmin_Password</t>
+  </si>
+  <si>
+    <t>Departmentscount</t>
+  </si>
+  <si>
+    <t>GroupByerrormessage</t>
+  </si>
+  <si>
+    <t>Please select atleast one value</t>
+  </si>
+  <si>
+    <t>todate</t>
+  </si>
+  <si>
+    <t>Reportname</t>
+  </si>
+  <si>
+    <t>UIAT</t>
+  </si>
+  <si>
+    <t>TimeperiodErrormessage</t>
+  </si>
+  <si>
+    <t>Please Select End Date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy&quot; &quot;hh&quot;:&quot;mm"/>
+    <numFmt numFmtId="166" formatCode="[$-14009]yyyy/mm/dd;@"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -869,7 +910,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
@@ -958,6 +999,8 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1739,7 +1782,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
@@ -1906,7 +1949,7 @@
       </c>
       <c r="E2" t="str">
         <f ca="1">"Testinguser"&amp;TEXT(NOW(),"ddmm")&amp;"@gmail.com"</f>
-        <v>Testinguser1910@gmail.com</v>
+        <v>Testinguser2010@gmail.com</v>
       </c>
       <c r="G2" t="s">
         <v>156</v>
@@ -1927,7 +1970,7 @@
       </c>
       <c r="E3" t="str">
         <f ca="1">"Testinguser"&amp;TEXT(NOW(),"ddmm")&amp;"@gmail.com"</f>
-        <v>Testinguser1910@gmail.com</v>
+        <v>Testinguser2010@gmail.com</v>
       </c>
       <c r="F3" t="s">
         <v>159</v>
@@ -1954,7 +1997,7 @@
       </c>
       <c r="E4" t="str">
         <f ca="1">"Testinguser"&amp;TEXT(NOW(),"ddmm")&amp;"@gmail.com"</f>
-        <v>Testinguser1910@gmail.com</v>
+        <v>Testinguser2010@gmail.com</v>
       </c>
       <c r="F4" t="s">
         <v>159</v>
@@ -2030,7 +2073,7 @@
       </c>
       <c r="E7" t="str">
         <f ca="1">"Testinguser"&amp;TEXT(NOW(),"ddmm")&amp;"@gmail.com"</f>
-        <v>Testinguser1910@gmail.com</v>
+        <v>Testinguser2010@gmail.com</v>
       </c>
       <c r="F7" t="s">
         <v>159</v>
@@ -2057,7 +2100,7 @@
       </c>
       <c r="E8" t="str">
         <f ca="1">"Testingspa"&amp;TEXT(NOW(),"ddmm")&amp;"@gmail.com"</f>
-        <v>Testingspa1910@gmail.com</v>
+        <v>Testingspa2010@gmail.com</v>
       </c>
       <c r="F8" t="s">
         <v>174</v>
@@ -2132,11 +2175,11 @@
       </c>
       <c r="D2" t="str">
         <f ca="1">"TestTeam"&amp;TEXT(NOW()+4,"ddmm")</f>
-        <v>TestTeam2310</v>
+        <v>TestTeam2410</v>
       </c>
       <c r="F2" t="str">
         <f ca="1">"Successfully created team : "&amp;D2</f>
-        <v>Successfully created team : TestTeam2310</v>
+        <v>Successfully created team : TestTeam2410</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -2151,7 +2194,7 @@
       </c>
       <c r="D3" t="str">
         <f ca="1">"TestTeam"&amp;TEXT(NOW()+4,"ddmm")</f>
-        <v>TestTeam2310</v>
+        <v>TestTeam2410</v>
       </c>
       <c r="F3" t="s">
         <v>183</v>
@@ -2170,7 +2213,7 @@
       </c>
       <c r="D4" t="str">
         <f ca="1">D2</f>
-        <v>TestTeam2310</v>
+        <v>TestTeam2410</v>
       </c>
       <c r="F4" t="s">
         <v>185</v>
@@ -2388,6 +2431,83 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="20.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E1" t="s">
+        <v>239</v>
+      </c>
+      <c r="F1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G1" t="s">
+        <v>242</v>
+      </c>
+      <c r="H1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>240</v>
+      </c>
+      <c r="F2" s="44"/>
+      <c r="G2" t="s">
+        <v>243</v>
+      </c>
+      <c r="H2" s="45" t="s">
+        <v>245</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2616,7 +2736,7 @@
       </c>
       <c r="M2" s="32">
         <f ca="1">NOW()+3</f>
-        <v>44126.896400810183</v>
+        <v>44127.963405555558</v>
       </c>
       <c r="N2" s="30" t="s">
         <v>11</v>
@@ -2833,10 +2953,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2844,6 +2964,7 @@
     <col min="1" max="1" width="21.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -2860,10 +2981,25 @@
         <v>122</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D2" t="s">
+        <v>235</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1"/>
     <hyperlink ref="D1" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Commit with custom reports cases on 04-11-2020
</commit_message>
<xml_diff>
--- a/TestData/IMIassist_Automation_TestData.xlsx
+++ b/TestData/IMIassist_Automation_TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="19" activeTab="20"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
     <sheet name="Login_testdata" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="277">
   <si>
     <t>URL</t>
   </si>
@@ -178,9 +178,6 @@
     <t>tikkinoknu@enayu.com</t>
   </si>
   <si>
-    <t>curzebispu@enayu.com</t>
-  </si>
-  <si>
     <t>Popup_Header</t>
   </si>
   <si>
@@ -394,10 +391,6 @@
     <t>Appointmentconfimrationtext</t>
   </si>
   <si>
-    <t xml:space="preserve">Appointment Scheduled Successfully
-</t>
-  </si>
-  <si>
     <t>9848321787</t>
   </si>
   <si>
@@ -431,27 +424,6 @@
     <t>IMIuuites</t>
   </si>
   <si>
-    <t>suatimate</t>
-  </si>
-  <si>
-    <t>suitimate</t>
-  </si>
-  <si>
-    <t>8912</t>
-  </si>
-  <si>
-    <t>+917829941767</t>
-  </si>
-  <si>
-    <t>imisuiauite@gmail.com</t>
-  </si>
-  <si>
-    <t>saiuimate</t>
-  </si>
-  <si>
-    <t>2016</t>
-  </si>
-  <si>
     <t>Invalidemail</t>
   </si>
   <si>
@@ -672,9 +644,6 @@
   </si>
   <si>
     <t>Chat History</t>
-  </si>
-  <si>
-    <t>test-879</t>
   </si>
   <si>
     <t>SupportadminUsername</t>
@@ -788,6 +757,129 @@
   </si>
   <si>
     <t>Please Select End Date</t>
+  </si>
+  <si>
+    <t>Appointmentlinktext</t>
+  </si>
+  <si>
+    <t>Start New Appointment</t>
+  </si>
+  <si>
+    <t>dultedukki@enayu.com</t>
+  </si>
+  <si>
+    <t>Appointmentcancelledsuccessfully</t>
+  </si>
+  <si>
+    <t>has been cancelled successfully</t>
+  </si>
+  <si>
+    <t>Team Name</t>
+  </si>
+  <si>
+    <t>Team Name attribute</t>
+  </si>
+  <si>
+    <t>Case ID</t>
+  </si>
+  <si>
+    <t>Case ID attribute</t>
+  </si>
+  <si>
+    <t>Appointment ID</t>
+  </si>
+  <si>
+    <t>Appointment ID attribute</t>
+  </si>
+  <si>
+    <t>Clinician Name attibute</t>
+  </si>
+  <si>
+    <t>Clinician Name</t>
+  </si>
+  <si>
+    <t>Patient Name attribute</t>
+  </si>
+  <si>
+    <t>Patient Name</t>
+  </si>
+  <si>
+    <t>Client ID attribute</t>
+  </si>
+  <si>
+    <t>Client ID</t>
+  </si>
+  <si>
+    <t>Patient Phone attribute</t>
+  </si>
+  <si>
+    <t>Patient Phone</t>
+  </si>
+  <si>
+    <t>Patient Email</t>
+  </si>
+  <si>
+    <t>Patient Email attrbite</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Notes attribute</t>
+  </si>
+  <si>
+    <t>Appointment Scheduled Successfully</t>
+  </si>
+  <si>
+    <t>addattributelinktext</t>
+  </si>
+  <si>
+    <t>Add filter</t>
+  </si>
+  <si>
+    <t>rafishaik</t>
+  </si>
+  <si>
+    <t>Invalidemailerror</t>
+  </si>
+  <si>
+    <t>Please enter valid email</t>
+  </si>
+  <si>
+    <t>castusork@enayu.com</t>
+  </si>
+  <si>
+    <t>test-939</t>
+  </si>
+  <si>
+    <t>suatimast</t>
+  </si>
+  <si>
+    <t>st</t>
+  </si>
+  <si>
+    <t>8915</t>
+  </si>
+  <si>
+    <t>+917889941768</t>
+  </si>
+  <si>
+    <t>imisuist@gmail.com</t>
+  </si>
+  <si>
+    <t>saiuist</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>Supportadmin</t>
+  </si>
+  <si>
+    <t>Supportadminpassword</t>
+  </si>
+  <si>
+    <t>Company Admin</t>
   </si>
 </sst>
 </file>
@@ -796,7 +888,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy&quot; &quot;hh&quot;:&quot;mm"/>
-    <numFmt numFmtId="166" formatCode="[$-14009]yyyy/mm/dd;@"/>
+    <numFmt numFmtId="165" formatCode="[$-14009]yyyy/mm/dd;@"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -910,7 +1002,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
@@ -999,8 +1091,11 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1369,10 +1464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1380,9 +1475,11 @@
     <col min="1" max="1" width="49.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1392,34 +1489,80 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>276</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2" location="!/registration/login" display="https://stg.imiassist.ai/agent/ - !/registration/login"/>
+    <hyperlink ref="C2" r:id="rId3"/>
+    <hyperlink ref="D2" r:id="rId4"/>
+    <hyperlink ref="D4" r:id="rId5"/>
+    <hyperlink ref="D3" r:id="rId6" display="mailto:tikkinoknu@enayu.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1450,7 +1593,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="28" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -1462,6 +1605,17 @@
         <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="29" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1471,6 +1625,7 @@
     <hyperlink ref="D2" r:id="rId2"/>
     <hyperlink ref="E2" r:id="rId3"/>
     <hyperlink ref="A2" r:id="rId4" location="!/registration/login"/>
+    <hyperlink ref="C4" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1478,10 +1633,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1513,26 +1668,26 @@
         <v>10</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="G1" s="37" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="A2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" s="29" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -1542,35 +1697,59 @@
         <v>9</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="G2" s="36" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="H2" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="I2" t="s">
-        <v>94</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2" location="!/registration/login"/>
-    <hyperlink ref="F2" r:id="rId3"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="C8" r:id="rId3"/>
+    <hyperlink ref="A8" r:id="rId4" location="!/registration/login"/>
+    <hyperlink ref="C2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId6"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1592,21 +1771,44 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B4" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="A2" r:id="rId3" location="!/registration/login"/>
+    <hyperlink ref="C7" r:id="rId2"/>
+    <hyperlink ref="B7" r:id="rId3"/>
+    <hyperlink ref="A7" r:id="rId4" location="!/registration/login"/>
+    <hyperlink ref="C4" r:id="rId5"/>
+    <hyperlink ref="B4" r:id="rId6"/>
+    <hyperlink ref="B2" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1614,16 +1816,16 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="49.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.26953125" customWidth="1"/>
+    <col min="2" max="2" width="26.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1639,21 +1841,33 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="A2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2"/>
-    <hyperlink ref="A2" r:id="rId3" location="!/registration/login"/>
+    <hyperlink ref="C7" r:id="rId1"/>
+    <hyperlink ref="B7" r:id="rId2"/>
+    <hyperlink ref="A7" r:id="rId3" location="!/registration/login"/>
+    <hyperlink ref="C2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1661,10 +1875,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1686,32 +1900,32 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>20</v>
+      <c r="A2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" t="s">
+        <v>132</v>
       </c>
       <c r="C2" s="29" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>142</v>
-      </c>
-      <c r="B3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C3" s="29" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="29" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2"/>
-    <hyperlink ref="A2" r:id="rId3" location="!/registration/login"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3" location="!/registration/login"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
@@ -1723,7 +1937,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1737,36 +1951,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="B1" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="C1" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>208</v>
+        <v>266</v>
       </c>
       <c r="B2" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D2" s="40" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E2" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -1782,8 +1996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1801,78 +2015,78 @@
   <sheetData>
     <row r="1" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="34" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="E1" s="34" t="s">
+        <v>209</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>211</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>213</v>
+      </c>
+      <c r="H1" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="I1" s="34" t="s">
+        <v>217</v>
+      </c>
+      <c r="J1" s="34" t="s">
         <v>219</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="K1" s="34" t="s">
         <v>221</v>
       </c>
-      <c r="G1" s="34" t="s">
-        <v>223</v>
-      </c>
-      <c r="H1" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="I1" s="34" t="s">
-        <v>227</v>
-      </c>
-      <c r="J1" s="34" t="s">
-        <v>229</v>
-      </c>
-      <c r="K1" s="34" t="s">
-        <v>231</v>
-      </c>
       <c r="L1" s="34" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="116" x14ac:dyDescent="0.35">
       <c r="A2" s="41" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="C2" s="41" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="D2" s="34">
         <v>8639183074</v>
       </c>
       <c r="E2" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="F2" s="42" t="s">
+        <v>212</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>214</v>
+      </c>
+      <c r="H2" s="34" t="s">
+        <v>216</v>
+      </c>
+      <c r="I2" s="34" t="s">
+        <v>218</v>
+      </c>
+      <c r="J2" s="43" t="s">
         <v>220</v>
-      </c>
-      <c r="F2" s="42" t="s">
-        <v>222</v>
-      </c>
-      <c r="G2" s="34" t="s">
-        <v>224</v>
-      </c>
-      <c r="H2" s="34" t="s">
-        <v>226</v>
-      </c>
-      <c r="I2" s="34" t="s">
-        <v>228</v>
-      </c>
-      <c r="J2" s="43" t="s">
-        <v>230</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>42</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1907,209 +2121,209 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="B2" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C2" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="D2" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="E2" t="str">
         <f ca="1">"Testinguser"&amp;TEXT(NOW(),"ddmm")&amp;"@gmail.com"</f>
-        <v>Testinguser2010@gmail.com</v>
+        <v>Testinguser2810@gmail.com</v>
       </c>
       <c r="G2" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="I2" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D3" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="E3" t="str">
         <f ca="1">"Testinguser"&amp;TEXT(NOW(),"ddmm")&amp;"@gmail.com"</f>
-        <v>Testinguser2010@gmail.com</v>
+        <v>Testinguser2810@gmail.com</v>
       </c>
       <c r="F3" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="G3" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="I3" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="B4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4" t="s">
         <v>153</v>
       </c>
-      <c r="C4" t="s">
-        <v>162</v>
-      </c>
       <c r="D4" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="E4" t="str">
         <f ca="1">"Testinguser"&amp;TEXT(NOW(),"ddmm")&amp;"@gmail.com"</f>
-        <v>Testinguser2010@gmail.com</v>
+        <v>Testinguser2810@gmail.com</v>
       </c>
       <c r="F4" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="G4" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="I4" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B5" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C5" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="D5" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="F5" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="G5" t="s">
+        <v>147</v>
+      </c>
+      <c r="I5" t="s">
         <v>156</v>
-      </c>
-      <c r="I5" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B6" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C6" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="D6" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="E6" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="F6" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="G6" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="H6" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="B7" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="C7" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="D7" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="E7" t="str">
         <f ca="1">"Testinguser"&amp;TEXT(NOW(),"ddmm")&amp;"@gmail.com"</f>
-        <v>Testinguser2010@gmail.com</v>
+        <v>Testinguser2810@gmail.com</v>
       </c>
       <c r="F7" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="G7" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="I7" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B8" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="C8" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D8" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="E8" t="str">
         <f ca="1">"Testingspa"&amp;TEXT(NOW(),"ddmm")&amp;"@gmail.com"</f>
-        <v>Testingspa2010@gmail.com</v>
+        <v>Testingspa2810@gmail.com</v>
       </c>
       <c r="F8" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="G8" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="I8" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -2121,8 +2335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2139,73 +2353,73 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="B2" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="C2" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="D2" t="str">
         <f ca="1">"TestTeam"&amp;TEXT(NOW()+4,"ddmm")</f>
-        <v>TestTeam2410</v>
+        <v>TestTeam0111</v>
       </c>
       <c r="F2" t="str">
         <f ca="1">"Successfully created team : "&amp;D2</f>
-        <v>Successfully created team : TestTeam2410</v>
+        <v>Successfully created team : TestTeam0111</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C3" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="D3" t="str">
         <f ca="1">"TestTeam"&amp;TEXT(NOW()+4,"ddmm")</f>
-        <v>TestTeam2410</v>
+        <v>TestTeam0111</v>
       </c>
       <c r="F3" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="B4" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="C4" t="str">
         <f>C2</f>
@@ -2213,16 +2427,16 @@
       </c>
       <c r="D4" t="str">
         <f ca="1">D2</f>
-        <v>TestTeam2410</v>
+        <v>TestTeam0111</v>
       </c>
       <c r="F4" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="G4" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="H4" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -2255,60 +2469,60 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="B2" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="C2" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="D2" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="E2" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="F2" s="39" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="G2" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="H2" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="I2" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -2352,7 +2566,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -2383,7 +2597,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2397,36 +2611,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="B2" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="C2" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="D2" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="E2" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -2436,10 +2650,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2450,40 +2664,78 @@
     <col min="5" max="5" width="19.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.08984375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="C1" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="D1" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="E1" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="F1" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="G1" t="s">
+        <v>232</v>
+      </c>
+      <c r="H1" t="s">
+        <v>234</v>
+      </c>
+      <c r="I1" t="s">
         <v>242</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>246</v>
+      </c>
+      <c r="L1" t="s">
+        <v>247</v>
+      </c>
+      <c r="M1" t="s">
+        <v>249</v>
+      </c>
+      <c r="N1" t="s">
+        <v>251</v>
+      </c>
+      <c r="O1" t="s">
+        <v>253</v>
+      </c>
+      <c r="P1" s="45" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q1" s="45" t="s">
+        <v>258</v>
+      </c>
+      <c r="R1" s="45" t="s">
+        <v>260</v>
+      </c>
+      <c r="S1" t="s">
+        <v>125</v>
+      </c>
+      <c r="T1" s="45" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>4</v>
@@ -2492,14 +2744,50 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="F2" s="44"/>
       <c r="G2" t="s">
+        <v>233</v>
+      </c>
+      <c r="H2" s="45" t="s">
+        <v>235</v>
+      </c>
+      <c r="I2" t="s">
+        <v>241</v>
+      </c>
+      <c r="J2" s="45" t="s">
         <v>243</v>
       </c>
-      <c r="H2" s="45" t="s">
+      <c r="K2" s="45" t="s">
         <v>245</v>
+      </c>
+      <c r="L2" s="45" t="s">
+        <v>248</v>
+      </c>
+      <c r="M2" s="45" t="s">
+        <v>250</v>
+      </c>
+      <c r="N2" s="45" t="s">
+        <v>252</v>
+      </c>
+      <c r="O2" s="45" t="s">
+        <v>254</v>
+      </c>
+      <c r="P2" s="45" t="s">
+        <v>255</v>
+      </c>
+      <c r="Q2" s="45" t="s">
+        <v>257</v>
+      </c>
+      <c r="R2" s="45" t="s">
+        <v>261</v>
+      </c>
+      <c r="S2" s="45" t="s">
+        <v>262</v>
+      </c>
+      <c r="T2" t="s">
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -2513,10 +2801,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2554,57 +2842,81 @@
         <v>18</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I1" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>126</v>
-      </c>
       <c r="E2" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>17</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2" location="!/registration/login" display="https://stg.imiassist.ai/agent/ - !/registration/login"/>
+    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3" location="!/registration/login" display="https://stg.imiassist.ai/agent/ - !/registration/login"/>
+    <hyperlink ref="C2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U6"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2632,7 +2944,7 @@
     <col min="21" max="16384" width="8.7265625" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" s="27" t="s">
         <v>19</v>
       </c>
@@ -2673,36 +2985,39 @@
         <v>32</v>
       </c>
       <c r="N1" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="O1" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="P1" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="P1" s="27" t="s">
-        <v>79</v>
-      </c>
       <c r="Q1" s="27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R1" s="27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S1" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="T1" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="T1" s="27" t="s">
-        <v>114</v>
-      </c>
       <c r="U1" s="27" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" s="30" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>20</v>
+        <v>116</v>
+      </c>
+      <c r="V1" s="27" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" s="30" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" t="s">
+        <v>132</v>
       </c>
       <c r="C2" s="29" t="s">
         <v>4</v>
@@ -2714,29 +3029,29 @@
         <v>4</v>
       </c>
       <c r="F2" s="30" t="s">
-        <v>127</v>
+        <v>267</v>
       </c>
       <c r="G2" s="30" t="s">
-        <v>128</v>
+        <v>268</v>
       </c>
       <c r="H2" s="30" t="s">
-        <v>129</v>
+        <v>269</v>
       </c>
       <c r="I2" s="30" t="s">
-        <v>130</v>
+        <v>270</v>
       </c>
       <c r="J2" s="31" t="s">
-        <v>131</v>
+        <v>271</v>
       </c>
       <c r="K2" s="30" t="s">
-        <v>132</v>
+        <v>272</v>
       </c>
       <c r="L2" s="30" t="s">
-        <v>133</v>
+        <v>273</v>
       </c>
       <c r="M2" s="32">
-        <f ca="1">NOW()+3</f>
-        <v>44127.963405555558</v>
+        <f ca="1">NOW()+2</f>
+        <v>44134.812106597223</v>
       </c>
       <c r="N2" s="30" t="s">
         <v>11</v>
@@ -2745,40 +3060,53 @@
         <v>3</v>
       </c>
       <c r="P2" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q2" s="33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="R2" s="30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S2" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T2" s="34" t="s">
+        <v>259</v>
+      </c>
+      <c r="U2" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="V2" s="30" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A3" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="U2" s="30" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="B6" s="30" t="s">
+      <c r="B3" s="30" t="s">
         <v>20</v>
       </c>
+      <c r="C3" s="29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B5" s="30"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="O2" r:id="rId4"/>
-    <hyperlink ref="J2" r:id="rId5"/>
-    <hyperlink ref="A2" r:id="rId6" location="!/registration/login"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="O2" r:id="rId3"/>
+    <hyperlink ref="J2" r:id="rId4"/>
+    <hyperlink ref="C3" r:id="rId5"/>
+    <hyperlink ref="A3" r:id="rId6" location="!/registration/login"/>
+    <hyperlink ref="C2" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -2787,7 +3115,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2797,13 +3125,13 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="35">
-        <f>DATE(2020,9,7)+1</f>
-        <v>44082</v>
+        <f>DATE(2020,9,7)+4</f>
+        <v>44085</v>
       </c>
     </row>
   </sheetData>
@@ -2842,72 +3170,72 @@
   <sheetData>
     <row r="1" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D1" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="22" t="s">
         <v>91</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>92</v>
       </c>
       <c r="F1" s="22" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H1" s="22" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J1" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="K1" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="L1" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="L1" s="22" t="s">
+      <c r="M1" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="M1" s="22" t="s">
-        <v>101</v>
-      </c>
       <c r="N1" s="22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O1" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="P1" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D2" s="20" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="21" t="s">
         <v>93</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>94</v>
       </c>
       <c r="G2" s="20" t="s">
         <v>42</v>
@@ -2916,10 +3244,10 @@
         <v>41</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K2" s="25">
         <v>43983</v>
@@ -2929,16 +3257,16 @@
         <v>44049</v>
       </c>
       <c r="M2" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="O2" s="26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="P2" s="21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2956,7 +3284,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2969,30 +3297,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="D2" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -3009,7 +3337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -3038,114 +3366,114 @@
   <sheetData>
     <row r="1" spans="1:19" s="13" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="13" t="s">
-        <v>48</v>
-      </c>
       <c r="F1" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H1" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="J1" s="13" t="s">
-        <v>59</v>
-      </c>
       <c r="K1" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N1" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="O1" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="P1" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="P1" s="13" t="s">
-        <v>69</v>
-      </c>
       <c r="Q1" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R1" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="S1" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="15" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="E2" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>51</v>
-      </c>
       <c r="F2" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J2" s="16" t="s">
         <v>3</v>
       </c>
       <c r="K2" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M2" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P2" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q2" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R2" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="S2" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -3159,10 +3487,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3173,7 +3501,7 @@
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3186,52 +3514,58 @@
       <c r="D1" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" s="4" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="28" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="28" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>43</v>
+        <v>115</v>
+      </c>
+      <c r="B4" s="46" t="s">
+        <v>238</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="28" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>20</v>
@@ -3243,9 +3577,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="28" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>3</v>
@@ -3264,9 +3598,9 @@
     <hyperlink ref="C5" r:id="rId3"/>
     <hyperlink ref="B6" r:id="rId4"/>
     <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="B4" r:id="rId6"/>
-    <hyperlink ref="A2" r:id="rId7" location="!/registration/login"/>
-    <hyperlink ref="A3:A6" r:id="rId8" location="!/registration/login" display="https://stg.imiassist.ai/agent/#!/registration/login"/>
+    <hyperlink ref="A2" r:id="rId6" location="!/registration/login"/>
+    <hyperlink ref="A3:A6" r:id="rId7" location="!/registration/login" display="https://stg.imiassist.ai/agent/#!/registration/login"/>
+    <hyperlink ref="B4" r:id="rId8" display="mailto:dultedukki@enayu.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId9"/>

</xml_diff>

<commit_message>
Code Changes on 24-1--2020
</commit_message>
<xml_diff>
--- a/TestData/IMIassist_Automation_TestData.xlsx
+++ b/TestData/IMIassist_Automation_TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Login_testdata" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="279">
   <si>
     <t>URL</t>
   </si>
@@ -880,6 +880,12 @@
   </si>
   <si>
     <t>Company Admin</t>
+  </si>
+  <si>
+    <t>TeamSearch</t>
+  </si>
+  <si>
+    <t>assigneduser</t>
   </si>
 </sst>
 </file>
@@ -1466,7 +1472,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -1937,7 +1943,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2163,7 +2169,7 @@
       </c>
       <c r="E2" t="str">
         <f ca="1">"Testinguser"&amp;TEXT(NOW(),"ddmm")&amp;"@gmail.com"</f>
-        <v>Testinguser2810@gmail.com</v>
+        <v>Testinguser2011@gmail.com</v>
       </c>
       <c r="G2" t="s">
         <v>147</v>
@@ -2184,7 +2190,7 @@
       </c>
       <c r="E3" t="str">
         <f ca="1">"Testinguser"&amp;TEXT(NOW(),"ddmm")&amp;"@gmail.com"</f>
-        <v>Testinguser2810@gmail.com</v>
+        <v>Testinguser2011@gmail.com</v>
       </c>
       <c r="F3" t="s">
         <v>150</v>
@@ -2211,7 +2217,7 @@
       </c>
       <c r="E4" t="str">
         <f ca="1">"Testinguser"&amp;TEXT(NOW(),"ddmm")&amp;"@gmail.com"</f>
-        <v>Testinguser2810@gmail.com</v>
+        <v>Testinguser2011@gmail.com</v>
       </c>
       <c r="F4" t="s">
         <v>150</v>
@@ -2287,7 +2293,7 @@
       </c>
       <c r="E7" t="str">
         <f ca="1">"Testinguser"&amp;TEXT(NOW(),"ddmm")&amp;"@gmail.com"</f>
-        <v>Testinguser2810@gmail.com</v>
+        <v>Testinguser2011@gmail.com</v>
       </c>
       <c r="F7" t="s">
         <v>150</v>
@@ -2314,7 +2320,7 @@
       </c>
       <c r="E8" t="str">
         <f ca="1">"Testingspa"&amp;TEXT(NOW(),"ddmm")&amp;"@gmail.com"</f>
-        <v>Testingspa2810@gmail.com</v>
+        <v>Testingspa2011@gmail.com</v>
       </c>
       <c r="F8" t="s">
         <v>165</v>
@@ -2389,11 +2395,11 @@
       </c>
       <c r="D2" t="str">
         <f ca="1">"TestTeam"&amp;TEXT(NOW()+4,"ddmm")</f>
-        <v>TestTeam0111</v>
+        <v>TestTeam2411</v>
       </c>
       <c r="F2" t="str">
         <f ca="1">"Successfully created team : "&amp;D2</f>
-        <v>Successfully created team : TestTeam0111</v>
+        <v>Successfully created team : TestTeam2411</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -2408,7 +2414,7 @@
       </c>
       <c r="D3" t="str">
         <f ca="1">"TestTeam"&amp;TEXT(NOW()+4,"ddmm")</f>
-        <v>TestTeam0111</v>
+        <v>TestTeam2411</v>
       </c>
       <c r="F3" t="s">
         <v>174</v>
@@ -2427,7 +2433,7 @@
       </c>
       <c r="D4" t="str">
         <f ca="1">D2</f>
-        <v>TestTeam0111</v>
+        <v>TestTeam2411</v>
       </c>
       <c r="F4" t="s">
         <v>176</v>
@@ -2913,10 +2919,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2941,10 +2947,12 @@
     <col min="18" max="18" width="35.08984375" style="27" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="17.81640625" style="27" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="26.08984375" style="27" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.7265625" style="27"/>
+    <col min="21" max="21" width="8.7265625" style="27"/>
+    <col min="22" max="22" width="29.7265625" style="27" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="8.7265625" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A1" s="27" t="s">
         <v>19</v>
       </c>
@@ -3011,13 +3019,19 @@
       <c r="V1" s="27" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" s="30" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B2" t="s">
-        <v>132</v>
+      <c r="W1" s="27" t="s">
+        <v>277</v>
+      </c>
+      <c r="X1" s="27" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" s="30" customFormat="1" ht="29" x14ac:dyDescent="0.2">
+      <c r="A2" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>20</v>
       </c>
       <c r="C2" s="29" t="s">
         <v>4</v>
@@ -3051,7 +3065,7 @@
       </c>
       <c r="M2" s="32">
         <f ca="1">NOW()+2</f>
-        <v>44134.812106597223</v>
+        <v>44157.78370821759</v>
       </c>
       <c r="N2" s="30" t="s">
         <v>11</v>
@@ -3080,8 +3094,14 @@
       <c r="V2" s="30" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W2" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="X2" s="45" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" s="28" t="s">
         <v>115</v>
       </c>
@@ -3092,7 +3112,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B5" s="30"/>
     </row>
   </sheetData>
@@ -3104,9 +3132,10 @@
     <hyperlink ref="C3" r:id="rId5"/>
     <hyperlink ref="A3" r:id="rId6" location="!/registration/login"/>
     <hyperlink ref="C2" r:id="rId7"/>
+    <hyperlink ref="A2" r:id="rId8" location="!/registration/login"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId9"/>
 </worksheet>
 </file>
 

</xml_diff>